<commit_message>
Update Add Module 4 assignments
</commit_message>
<xml_diff>
--- a/module-4/assignment-1.xlsx
+++ b/module-4/assignment-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\csd\csd-380\module-4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6BDF5838-74DA-416B-A07F-B090D5F4F13E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9A42CBD-6E49-40A7-89D7-A3E69A10410F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22884" yWindow="2052" windowWidth="27180" windowHeight="16980" xr2:uid="{72852274-8636-4B6E-8714-77761460E6D6}"/>
+    <workbookView xWindow="5690" yWindow="3230" windowWidth="23040" windowHeight="12370" xr2:uid="{72852274-8636-4B6E-8714-77761460E6D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -205,7 +205,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="67">
   <si>
     <t>Test 1</t>
   </si>
@@ -552,12 +552,15 @@
   <si>
     <t>The application adjusted well to mobile secreen sized without major issues and no issues found with scrolling or UI layout. Editing tasks on the different devices were functional and ran without any issues.</t>
   </si>
+  <si>
+    <t>https://github.com/VanhSom/csd-380.git</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -624,6 +627,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -803,7 +814,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -841,6 +852,57 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -850,60 +912,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1394,60 +1406,63 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="30"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="23"/>
     </row>
     <row r="2" spans="1:6" ht="23" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="16"/>
-      <c r="B2" s="18" t="s">
+      <c r="A2" s="24"/>
+      <c r="B2" s="19" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="21"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="34" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="17"/>
-      <c r="B3" s="19"/>
+      <c r="A3" s="25"/>
+      <c r="B3" s="20"/>
       <c r="C3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="E3" s="23"/>
+      <c r="E3" s="29"/>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="31" t="s">
+      <c r="E4" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="32"/>
+      <c r="F4" s="14"/>
     </row>
     <row r="5" spans="1:6" ht="11" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="19"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
+      <c r="A5" s="20"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
       <c r="E5" s="8" t="s">
         <v>9</v>
       </c>
@@ -1517,48 +1532,48 @@
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="15"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="32"/>
     </row>
     <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="11" spans="1:6" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="30"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="23"/>
     </row>
     <row r="12" spans="1:6" ht="23" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="16"/>
-      <c r="B12" s="18" t="s">
+      <c r="A12" s="24"/>
+      <c r="B12" s="19" t="s">
         <v>21</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="E12" s="21"/>
+      <c r="E12" s="27"/>
     </row>
     <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="17"/>
-      <c r="B13" s="19"/>
+      <c r="A13" s="25"/>
+      <c r="B13" s="20"/>
       <c r="C13" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="D13" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="23"/>
+      <c r="E13" s="29"/>
     </row>
     <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="3" t="s">
@@ -1641,48 +1656,48 @@
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="15"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="32"/>
     </row>
     <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="20" spans="1:6" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="28" t="s">
+      <c r="B20" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="30"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="23"/>
     </row>
     <row r="21" spans="1:6" ht="23" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="16"/>
-      <c r="B21" s="18" t="s">
+      <c r="A21" s="24"/>
+      <c r="B21" s="19" t="s">
         <v>30</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="20" t="s">
+      <c r="D21" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="E21" s="21"/>
+      <c r="E21" s="27"/>
     </row>
     <row r="22" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="17"/>
-      <c r="B22" s="19"/>
+      <c r="A22" s="25"/>
+      <c r="B22" s="20"/>
       <c r="C22" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D22" s="22" t="s">
+      <c r="D22" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="E22" s="23"/>
+      <c r="E22" s="29"/>
     </row>
     <row r="23" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="3" t="s">
@@ -1717,7 +1732,7 @@
       <c r="E24" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F24" s="33" t="e" vm="7">
+      <c r="F24" s="15" t="e" vm="7">
         <v>#VALUE!</v>
       </c>
     </row>
@@ -1765,48 +1780,48 @@
       <c r="A27" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="15"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="32"/>
     </row>
     <row r="28" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="29" spans="1:6" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="28" t="s">
+      <c r="B29" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="30"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="23"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" s="16"/>
-      <c r="B30" s="18" t="s">
+      <c r="A30" s="24"/>
+      <c r="B30" s="19" t="s">
         <v>40</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D30" s="20" t="s">
+      <c r="D30" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="E30" s="21"/>
+      <c r="E30" s="27"/>
     </row>
     <row r="31" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="17"/>
-      <c r="B31" s="19"/>
+      <c r="A31" s="25"/>
+      <c r="B31" s="20"/>
       <c r="C31" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="22" t="s">
+      <c r="D31" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="E31" s="23"/>
+      <c r="E31" s="29"/>
     </row>
     <row r="32" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="3" t="s">
@@ -1841,45 +1856,45 @@
       <c r="E33" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F33" s="33" t="e" vm="10">
+      <c r="F33" s="15" t="e" vm="10">
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="25" x14ac:dyDescent="0.35">
-      <c r="A34" s="16">
+      <c r="A34" s="24">
         <v>2</v>
       </c>
       <c r="B34" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C34" s="25" t="s">
+      <c r="C34" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="D34" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="E34" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="F34" s="25" t="e" vm="11">
+      <c r="D34" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34" s="16" t="e" vm="11">
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" s="24"/>
+      <c r="A35" s="33"/>
       <c r="B35" s="11"/>
-      <c r="C35" s="26"/>
-      <c r="D35" s="26"/>
-      <c r="E35" s="26"/>
-      <c r="F35" s="26"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
     </row>
     <row r="36" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="17"/>
+      <c r="A36" s="25"/>
       <c r="B36" s="12"/>
-      <c r="C36" s="27"/>
-      <c r="D36" s="27"/>
-      <c r="E36" s="27"/>
-      <c r="F36" s="27"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
     </row>
     <row r="37" spans="1:6" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="2">
@@ -1905,48 +1920,48 @@
       <c r="A38" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B38" s="13" t="s">
+      <c r="B38" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="15"/>
+      <c r="C38" s="31"/>
+      <c r="D38" s="31"/>
+      <c r="E38" s="32"/>
     </row>
     <row r="39" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="40" spans="1:6" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B40" s="28" t="s">
+      <c r="B40" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="C40" s="29"/>
-      <c r="D40" s="29"/>
-      <c r="E40" s="30"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="23"/>
     </row>
     <row r="41" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="16"/>
-      <c r="B41" s="18" t="s">
+      <c r="A41" s="24"/>
+      <c r="B41" s="19" t="s">
         <v>50</v>
       </c>
       <c r="C41" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D41" s="20" t="s">
+      <c r="D41" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="E41" s="21"/>
+      <c r="E41" s="27"/>
     </row>
     <row r="42" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="17"/>
-      <c r="B42" s="19"/>
+      <c r="A42" s="25"/>
+      <c r="B42" s="20"/>
       <c r="C42" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D42" s="22" t="s">
+      <c r="D42" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="E42" s="23"/>
+      <c r="E42" s="29"/>
     </row>
     <row r="43" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="3" t="s">
@@ -1981,45 +1996,45 @@
       <c r="E44" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F44" s="33" t="e" vm="13">
+      <c r="F44" s="15" t="e" vm="13">
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="16">
+      <c r="A45" s="24">
         <v>2</v>
       </c>
       <c r="B45" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C45" s="25" t="s">
+      <c r="C45" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="D45" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="E45" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="F45" s="25" t="e" vm="14">
+      <c r="D45" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E45" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F45" s="16" t="e" vm="14">
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="24"/>
+      <c r="A46" s="33"/>
       <c r="B46" s="11"/>
-      <c r="C46" s="26"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="26"/>
-      <c r="F46" s="26"/>
+      <c r="C46" s="17"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="17"/>
     </row>
     <row r="47" spans="1:6" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="17"/>
+      <c r="A47" s="25"/>
       <c r="B47" s="12"/>
-      <c r="C47" s="27"/>
-      <c r="D47" s="27"/>
-      <c r="E47" s="27"/>
-      <c r="F47" s="27"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="18"/>
     </row>
     <row r="48" spans="1:6" ht="66.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="2">
@@ -2045,26 +2060,49 @@
       <c r="A49" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B49" s="13" t="s">
+      <c r="B49" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="15"/>
+      <c r="C49" s="31"/>
+      <c r="D49" s="31"/>
+      <c r="E49" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="44">
+    <mergeCell ref="B49:E49"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="C45:C47"/>
+    <mergeCell ref="D45:D47"/>
+    <mergeCell ref="E45:E47"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="E34:E36"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B38:E38"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
     <mergeCell ref="F45:F47"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="F34:F36"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B11:E11"/>
     <mergeCell ref="A12:A13"/>
@@ -2075,29 +2113,6 @@
     <mergeCell ref="B20:E20"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="B21:B22"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="B40:E40"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="C34:C36"/>
-    <mergeCell ref="D34:D36"/>
-    <mergeCell ref="E34:E36"/>
-    <mergeCell ref="B38:E38"/>
-    <mergeCell ref="B49:E49"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="C45:C47"/>
-    <mergeCell ref="D45:D47"/>
-    <mergeCell ref="E45:E47"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" display="https://buwebdev.github.io/todo/" xr:uid="{63C4EA35-36D1-4C2D-BAB3-C03F0B5AC7FD}"/>

</xml_diff>